<commit_message>
First functioning solution; needs to be beautified/finalized.
</commit_message>
<xml_diff>
--- a/SwissQRBill.xlsx
+++ b/SwissQRBill.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{861709F2-9A8A-4B21-81A6-86EBF11AE260}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD6172F3-05C7-4D77-A145-F0A1502B2016}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SwissQRCode (old)" sheetId="3" state="hidden" r:id="rId1"/>
@@ -71,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="432" uniqueCount="228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="467" uniqueCount="238">
   <si>
     <t>Empfangsschein</t>
   </si>
@@ -836,6 +836,36 @@
   </si>
   <si>
     <t>Document generated! 28 bookmarks replaced. Path =C:\Users\imfeldc\source\repos\SwissQRCodeExcel4\zz Rechnungs Test Vorlage - Automatisiert.docx at 03.01.2021 18:58:57</t>
+  </si>
+  <si>
+    <t>QR Template</t>
+  </si>
+  <si>
+    <t>C:\Users\imfeldc\source\repos\SwissQRCodeExcel4\zz Rechnungs Test Vorlage - Automatisiert.docx</t>
+  </si>
+  <si>
+    <t>(A29)</t>
+  </si>
+  <si>
+    <t>generateDocument: Document generated! 28 bookmarks replaced. Path =C:\Users\imfeldc\source\repos\SwissQRCodeExcel4\zz Rechnungs Test Vorlage - Automatisiert.docx at 04.01.2021 10:36:20</t>
+  </si>
+  <si>
+    <t>QR Code generated! Path=C:\Users\imfeldc\AppData\Local\Temp\qrcode.bmp / AltPath=C:\Users\imfeldc\source\repos\SwissQRCodeExcel4\qrcode.bmp at 04.01.2021 10:37:07</t>
+  </si>
+  <si>
+    <t>generateDocument: Document generated! 28 bookmarks replaced. Path =C:\Users\imfeldc\source\repos\SwissQRCodeExcel4\zz Rechnungs Test Vorlage - Automatisiert.docx at 04.01.2021 10:59:22</t>
+  </si>
+  <si>
+    <t>QR Code generated! Path=C:\Users\imfeldc\AppData\Local\Temp\qrcode.bmp / AltPath=C:\Users\imfeldc\source\repos\SwissQRCodeExcel4\qrcode.bmp at 04.01.2021 10:59:37</t>
+  </si>
+  <si>
+    <t>QR Code generated! Path=C:\Users\imfeldc\AppData\Local\Temp\qrcode.bmp / AltPath=C:\Users\imfeldc\source\repos\SwissQRCodeExcel4\qrcode.bmp at 04.01.2021 11:00:11</t>
+  </si>
+  <si>
+    <t>QR Code generated! Path=C:\Users\imfeldc\AppData\Local\Temp\qrcode.bmp / AltPath=C:\Users\imfeldc\source\repos\SwissQRCodeExcel4\qrcode.bmp at 04.01.2021 11:00:33</t>
+  </si>
+  <si>
+    <t>QR Code generated! Path=C:\Users\imfeldc\AppData\Local\Temp\qrcode.bmp / AltPath=C:\Users\imfeldc\source\repos\SwissQRCodeExcel4\qrcode.bmp at 04.01.2021 11:00:43</t>
   </si>
 </sst>
 </file>
@@ -1887,13 +1917,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>1052497</xdr:colOff>
-      <xdr:row>27</xdr:row>
+      <xdr:row>30</xdr:row>
       <xdr:rowOff>33326</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>1071547</xdr:colOff>
-      <xdr:row>47</xdr:row>
+      <xdr:row>50</xdr:row>
       <xdr:rowOff>98576</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1940,13 +1970,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>4760</xdr:colOff>
-      <xdr:row>27</xdr:row>
+      <xdr:row>30</xdr:row>
       <xdr:rowOff>38088</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>592460</xdr:colOff>
-      <xdr:row>27</xdr:row>
+      <xdr:row>30</xdr:row>
       <xdr:rowOff>47625</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1993,13 +2023,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>47</xdr:row>
+      <xdr:row>50</xdr:row>
       <xdr:rowOff>90488</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>1069950</xdr:colOff>
-      <xdr:row>47</xdr:row>
+      <xdr:row>50</xdr:row>
       <xdr:rowOff>90497</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -2046,13 +2076,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>1076369</xdr:colOff>
-      <xdr:row>47</xdr:row>
+      <xdr:row>50</xdr:row>
       <xdr:rowOff>90485</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>585788</xdr:colOff>
-      <xdr:row>47</xdr:row>
+      <xdr:row>50</xdr:row>
       <xdr:rowOff>90488</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -2099,13 +2129,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>9526</xdr:colOff>
-      <xdr:row>38</xdr:row>
+      <xdr:row>41</xdr:row>
       <xdr:rowOff>100013</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>871538</xdr:colOff>
-      <xdr:row>38</xdr:row>
+      <xdr:row>41</xdr:row>
       <xdr:rowOff>100019</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -2152,13 +2182,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>14287</xdr:colOff>
-      <xdr:row>29</xdr:row>
+      <xdr:row>32</xdr:row>
       <xdr:rowOff>161927</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>876299</xdr:colOff>
-      <xdr:row>29</xdr:row>
+      <xdr:row>32</xdr:row>
       <xdr:rowOff>161933</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -2205,13 +2235,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>9524</xdr:colOff>
-      <xdr:row>29</xdr:row>
+      <xdr:row>32</xdr:row>
       <xdr:rowOff>157169</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>38</xdr:row>
+      <xdr:row>41</xdr:row>
       <xdr:rowOff>104775</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -2258,13 +2288,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>866775</xdr:colOff>
-      <xdr:row>29</xdr:row>
+      <xdr:row>32</xdr:row>
       <xdr:rowOff>166688</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>876300</xdr:colOff>
-      <xdr:row>38</xdr:row>
+      <xdr:row>41</xdr:row>
       <xdr:rowOff>100013</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -2307,25 +2337,30 @@
     </xdr:cxnSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>1136650</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>254000</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>1200150</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>120650</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>3048000</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="7" name="Picture 6">
+        <xdr:cNvPr id="8" name="Picture 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6A267769-D44A-4E61-A30C-749270DCACE8}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{72CB6ADC-0A12-4787-A1EA-66F8F3D45ED9}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2347,8 +2382,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2222500" y="5715000"/>
-          <a:ext cx="1778000" cy="1778000"/>
+          <a:off x="254000" y="254000"/>
+          <a:ext cx="2794000" cy="2794000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2357,11 +2392,6 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
@@ -2377,10 +2407,10 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2">
+        <xdr:cNvPr id="10" name="Picture 9">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9680F30B-62A8-427E-A19D-FFE85A88ED98}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6C19A240-D4E6-4108-8FAD-9F4AA0F59687}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -17720,10 +17750,10 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:G52"/>
+  <dimension ref="A1:G55"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E47" sqref="E47"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17900,7 +17930,7 @@
         <v>54</v>
       </c>
       <c r="B22" s="9">
-        <v>450</v>
+        <v>490</v>
       </c>
       <c r="D22" t="s">
         <v>74</v>
@@ -17942,223 +17972,239 @@
         <v>79</v>
       </c>
     </row>
-    <row r="28" spans="1:6" s="1" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="F28" s="2"/>
-    </row>
-    <row r="29" spans="1:6" s="1" customFormat="1" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A29" s="3" t="s">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="9"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="5" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="9" t="s">
+        <v>229</v>
+      </c>
+      <c r="D29" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" s="1" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="F31" s="2"/>
+    </row>
+    <row r="32" spans="1:6" s="1" customFormat="1" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="A32" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B29" s="3"/>
-      <c r="C29" s="4"/>
-      <c r="D29" s="3" t="s">
+      <c r="B32" s="3"/>
+      <c r="C32" s="4"/>
+      <c r="D32" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="F29" s="5" t="s">
+      <c r="F32" s="5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="1:6" s="1" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A30" s="6" t="s">
+    <row r="33" spans="1:7" s="1" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A33" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="F30" s="16" t="str">
-        <f>A31</f>
+      <c r="F33" s="16" t="str">
+        <f>A34</f>
         <v>CH04 3078 7007 7190 5090 2</v>
       </c>
     </row>
-    <row r="31" spans="1:6" s="7" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A31" s="7" t="str">
+    <row r="34" spans="1:7" s="7" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A34" s="7" t="str">
         <f>A2</f>
         <v>CH04 3078 7007 7190 5090 2</v>
       </c>
-      <c r="B31" s="5"/>
-      <c r="F31" s="16" t="str">
-        <f>A32</f>
+      <c r="B34" s="5"/>
+      <c r="F34" s="16" t="str">
+        <f>A35</f>
         <v>fotoleu</v>
       </c>
     </row>
-    <row r="32" spans="1:6" s="1" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A32" s="7" t="str">
+    <row r="35" spans="1:7" s="1" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A35" s="7" t="str">
         <f>A3</f>
         <v>fotoleu</v>
       </c>
-      <c r="B32" s="2"/>
-      <c r="F32" s="16" t="str">
-        <f>A33</f>
+      <c r="B35" s="2"/>
+      <c r="F35" s="16" t="str">
+        <f>A36</f>
         <v>Inh. Anita Imfeld-Leu</v>
       </c>
     </row>
-    <row r="33" spans="1:7" s="1" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A33" s="7" t="str">
+    <row r="36" spans="1:7" s="1" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A36" s="7" t="str">
         <f>A4</f>
         <v>Inh. Anita Imfeld-Leu</v>
       </c>
-      <c r="B33" s="2"/>
-      <c r="F33" s="16" t="str">
-        <f>A34</f>
+      <c r="B36" s="2"/>
+      <c r="F36" s="16" t="str">
+        <f>A37</f>
         <v>Bösch 63, 6331 Hünenberg</v>
       </c>
     </row>
-    <row r="34" spans="1:7" s="1" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A34" s="7" t="str">
+    <row r="37" spans="1:7" s="1" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A37" s="7" t="str">
         <f>A5</f>
         <v>Bösch 63, 6331 Hünenberg</v>
       </c>
-      <c r="B34" s="2"/>
-      <c r="F34" s="2"/>
-    </row>
-    <row r="35" spans="1:7" s="1" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A35" s="7"/>
-      <c r="F35" s="5" t="s">
+      <c r="B37" s="2"/>
+      <c r="F37" s="2"/>
+    </row>
+    <row r="38" spans="1:7" s="1" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A38" s="7"/>
+      <c r="F38" s="5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="36" spans="1:7" s="1" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A36" s="6" t="s">
+    <row r="39" spans="1:7" s="1" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A39" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="F36" s="2" t="str">
+      <c r="F39" s="2" t="str">
         <f>A8</f>
         <v>KF1515</v>
       </c>
     </row>
-    <row r="37" spans="1:7" s="1" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A37" s="7" t="str">
+    <row r="40" spans="1:7" s="1" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A40" s="7" t="str">
         <f>A12</f>
         <v>Christian Imfeld</v>
       </c>
-      <c r="B37" s="5"/>
-      <c r="F37" s="2" t="str">
+      <c r="B40" s="5"/>
+      <c r="F40" s="2" t="str">
         <f>A9</f>
         <v>Datum 01.10.2020</v>
       </c>
-      <c r="G37" s="8"/>
-    </row>
-    <row r="38" spans="1:7" s="1" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A38" s="7" t="str">
+      <c r="G40" s="8"/>
+    </row>
+    <row r="41" spans="1:7" s="1" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A41" s="7" t="str">
         <f>A13</f>
         <v>Eichholzweg 9</v>
       </c>
-      <c r="B38" s="2"/>
-      <c r="F38" s="2"/>
-    </row>
-    <row r="39" spans="1:7" s="1" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A39" s="7" t="str">
+      <c r="B41" s="2"/>
+      <c r="F41" s="2"/>
+    </row>
+    <row r="42" spans="1:7" s="1" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A42" s="7" t="str">
         <f>A14</f>
         <v>6312 Steinhausen</v>
       </c>
-      <c r="B39" s="2"/>
-      <c r="F39" s="5" t="s">
+      <c r="B42" s="2"/>
+      <c r="F42" s="5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="40" spans="1:7" s="1" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A40" s="7"/>
-      <c r="B40" s="5"/>
-      <c r="F40" s="16" t="str">
-        <f>A37</f>
+    <row r="43" spans="1:7" s="1" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A43" s="7"/>
+      <c r="B43" s="5"/>
+      <c r="F43" s="16" t="str">
+        <f>A40</f>
         <v>Christian Imfeld</v>
       </c>
     </row>
-    <row r="41" spans="1:7" s="1" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A41" s="6" t="s">
+    <row r="44" spans="1:7" s="1" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A44" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B41" s="6" t="s">
+      <c r="B44" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D41" s="5" t="s">
+      <c r="D44" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="E41" s="5" t="s">
+      <c r="E44" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="F41" s="16" t="str">
-        <f>A38</f>
+      <c r="F44" s="16" t="str">
+        <f>A41</f>
         <v>Eichholzweg 9</v>
       </c>
     </row>
-    <row r="42" spans="1:7" s="1" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A42" s="7" t="str">
+    <row r="45" spans="1:7" s="1" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A45" s="7" t="str">
         <f>A18</f>
         <v>CHF</v>
       </c>
-      <c r="B42" s="9">
+      <c r="B45" s="9">
         <f>A17</f>
         <v>12</v>
       </c>
-      <c r="D42" s="2" t="str">
+      <c r="D45" s="2" t="str">
         <f>A18</f>
         <v>CHF</v>
       </c>
-      <c r="E42" s="17">
+      <c r="E45" s="17">
         <f>A17</f>
         <v>12</v>
       </c>
-      <c r="F42" s="16" t="str">
-        <f>A39</f>
+      <c r="F45" s="16" t="str">
+        <f>A42</f>
         <v>6312 Steinhausen</v>
       </c>
     </row>
-    <row r="43" spans="1:7" s="1" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A43" s="7"/>
-      <c r="B43" s="9"/>
-      <c r="D43" s="2"/>
-      <c r="E43" s="10"/>
-      <c r="F43" s="2"/>
-    </row>
-    <row r="44" spans="1:7" s="1" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A44" s="11"/>
-      <c r="B44"/>
-      <c r="C44" s="12" t="s">
+    <row r="46" spans="1:7" s="1" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A46" s="7"/>
+      <c r="B46" s="9"/>
+      <c r="D46" s="2"/>
+      <c r="E46" s="10"/>
+      <c r="F46" s="2"/>
+    </row>
+    <row r="47" spans="1:7" s="1" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A47" s="11"/>
+      <c r="B47"/>
+      <c r="C47" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="D44"/>
-      <c r="F44" s="2"/>
-    </row>
-    <row r="45" spans="1:7" s="1" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="B45" s="11"/>
-      <c r="D45"/>
-      <c r="E45"/>
-      <c r="F45" s="2"/>
-    </row>
-    <row r="46" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A46"/>
-      <c r="F46" s="2"/>
-    </row>
-    <row r="47" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A47"/>
-      <c r="B47"/>
-      <c r="C47"/>
       <c r="D47"/>
-      <c r="E47"/>
       <c r="F47" s="2"/>
     </row>
-    <row r="48" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A48" s="11"/>
-    </row>
-    <row r="49" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A49" s="11"/>
-      <c r="B49" s="11"/>
-    </row>
-    <row r="50" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A50" s="14"/>
-      <c r="B50" s="11"/>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B51" s="14"/>
-      <c r="C51" s="14"/>
-      <c r="D51" s="14"/>
-      <c r="E51" s="14"/>
-    </row>
-    <row r="52" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A52"/>
-      <c r="B52"/>
-      <c r="C52"/>
-      <c r="D52"/>
-      <c r="E52"/>
-      <c r="F52" s="15"/>
+    <row r="48" spans="1:7" s="1" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="B48" s="11"/>
+      <c r="D48"/>
+      <c r="E48"/>
+      <c r="F48" s="2"/>
+    </row>
+    <row r="49" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A49"/>
+      <c r="F49" s="2"/>
+    </row>
+    <row r="50" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A50"/>
+      <c r="B50"/>
+      <c r="C50"/>
+      <c r="D50"/>
+      <c r="E50"/>
+      <c r="F50" s="2"/>
+    </row>
+    <row r="51" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A51" s="11"/>
+    </row>
+    <row r="52" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A52" s="11"/>
+      <c r="B52" s="11"/>
+    </row>
+    <row r="53" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A53" s="14"/>
+      <c r="B53" s="11"/>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B54" s="14"/>
+      <c r="C54" s="14"/>
+      <c r="D54" s="14"/>
+      <c r="E54" s="14"/>
+    </row>
+    <row r="55" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A55"/>
+      <c r="B55"/>
+      <c r="C55"/>
+      <c r="D55"/>
+      <c r="E55"/>
+      <c r="F55" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -18169,9 +18215,9 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4C13067-15AF-4F78-98EF-8797820B2B84}">
-  <dimension ref="A2:H54"/>
+  <dimension ref="A2:H61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
@@ -18260,57 +18306,97 @@
       <c r="G19" s="21"/>
       <c r="H19" s="21"/>
     </row>
-    <row r="20" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A20" s="20" t="s">
-        <v>227</v>
-      </c>
-      <c r="B20" s="22"/>
-      <c r="C20" s="22"/>
-      <c r="D20" s="22"/>
-      <c r="E20" s="22"/>
-      <c r="F20" s="22"/>
+        <v>237</v>
+      </c>
+      <c r="B20" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="C20" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="D20" s="22" t="s">
+        <v>49</v>
+      </c>
+      <c r="E20" s="22" t="s">
+        <v>71</v>
+      </c>
+      <c r="F20" s="22" t="s">
+        <v>45</v>
+      </c>
       <c r="G20" s="21"/>
       <c r="H20" s="21"/>
     </row>
-    <row r="21" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A21" s="20" t="s">
-        <v>226</v>
-      </c>
-      <c r="B21" s="22"/>
-      <c r="C21" s="22"/>
-      <c r="D21" s="22"/>
-      <c r="E21" s="22"/>
-      <c r="F21" s="22"/>
+        <v>236</v>
+      </c>
+      <c r="B21" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="C21" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="D21" s="22" t="s">
+        <v>49</v>
+      </c>
+      <c r="E21" s="22" t="s">
+        <v>71</v>
+      </c>
+      <c r="F21" s="22" t="s">
+        <v>45</v>
+      </c>
       <c r="G21" s="21"/>
       <c r="H21" s="21"/>
     </row>
-    <row r="22" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A22" s="20" t="s">
-        <v>224</v>
-      </c>
-      <c r="B22" s="22"/>
-      <c r="C22" s="22"/>
-      <c r="D22" s="22"/>
-      <c r="E22" s="22"/>
-      <c r="F22" s="22"/>
+        <v>235</v>
+      </c>
+      <c r="B22" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="C22" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="D22" s="22" t="s">
+        <v>49</v>
+      </c>
+      <c r="E22" s="22" t="s">
+        <v>71</v>
+      </c>
+      <c r="F22" s="22" t="s">
+        <v>45</v>
+      </c>
       <c r="G22" s="21"/>
       <c r="H22" s="21"/>
     </row>
-    <row r="23" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A23" s="20" t="s">
-        <v>222</v>
-      </c>
-      <c r="B23" s="22"/>
-      <c r="C23" s="22"/>
-      <c r="D23" s="22"/>
-      <c r="E23" s="22"/>
-      <c r="F23" s="22"/>
+        <v>234</v>
+      </c>
+      <c r="B23" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="C23" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="D23" s="22" t="s">
+        <v>49</v>
+      </c>
+      <c r="E23" s="22" t="s">
+        <v>71</v>
+      </c>
+      <c r="F23" s="22" t="s">
+        <v>45</v>
+      </c>
       <c r="G23" s="21"/>
       <c r="H23" s="21"/>
     </row>
-    <row r="24" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A24" s="20" t="s">
-        <v>221</v>
+        <v>233</v>
       </c>
       <c r="B24" s="22"/>
       <c r="C24" s="22"/>
@@ -18320,175 +18406,115 @@
       <c r="G24" s="21"/>
       <c r="H24" s="21"/>
     </row>
-    <row r="25" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A25" s="20" t="s">
-        <v>220</v>
-      </c>
-      <c r="B25" s="22"/>
-      <c r="C25" s="22"/>
-      <c r="D25" s="22"/>
-      <c r="E25" s="22"/>
-      <c r="F25" s="22"/>
+        <v>232</v>
+      </c>
+      <c r="B25" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="C25" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="D25" s="22" t="s">
+        <v>49</v>
+      </c>
+      <c r="E25" s="22" t="s">
+        <v>71</v>
+      </c>
+      <c r="F25" s="22" t="s">
+        <v>45</v>
+      </c>
       <c r="G25" s="21"/>
       <c r="H25" s="21"/>
     </row>
-    <row r="26" spans="1:8" ht="120" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A26" s="20" t="s">
-        <v>94</v>
-      </c>
-      <c r="B26" s="22" t="s">
-        <v>35</v>
-      </c>
-      <c r="C26" s="22" t="s">
-        <v>36</v>
-      </c>
-      <c r="D26" s="22" t="s">
-        <v>49</v>
-      </c>
-      <c r="E26" s="22" t="s">
-        <v>71</v>
-      </c>
-      <c r="F26" s="22" t="s">
-        <v>45</v>
-      </c>
+        <v>231</v>
+      </c>
+      <c r="B26" s="22"/>
+      <c r="C26" s="22"/>
+      <c r="D26" s="22"/>
+      <c r="E26" s="22"/>
+      <c r="F26" s="22"/>
       <c r="G26" s="21"/>
       <c r="H26" s="21"/>
     </row>
-    <row r="27" spans="1:8" ht="120" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A27" s="20" t="s">
-        <v>93</v>
-      </c>
-      <c r="B27" s="22" t="s">
-        <v>35</v>
-      </c>
-      <c r="C27" s="22" t="s">
-        <v>36</v>
-      </c>
-      <c r="D27" s="22" t="s">
-        <v>49</v>
-      </c>
-      <c r="E27" s="22" t="s">
-        <v>71</v>
-      </c>
-      <c r="F27" s="22" t="s">
-        <v>45</v>
-      </c>
+        <v>227</v>
+      </c>
+      <c r="B27" s="22"/>
+      <c r="C27" s="22"/>
+      <c r="D27" s="22"/>
+      <c r="E27" s="22"/>
+      <c r="F27" s="22"/>
       <c r="G27" s="21"/>
       <c r="H27" s="21"/>
     </row>
-    <row r="28" spans="1:8" ht="120" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A28" s="20" t="s">
-        <v>92</v>
-      </c>
-      <c r="B28" s="22" t="s">
-        <v>35</v>
-      </c>
-      <c r="C28" s="22" t="s">
-        <v>36</v>
-      </c>
-      <c r="D28" s="22" t="s">
-        <v>49</v>
-      </c>
-      <c r="E28" s="22" t="s">
-        <v>71</v>
-      </c>
-      <c r="F28" s="22" t="s">
-        <v>45</v>
-      </c>
+        <v>226</v>
+      </c>
+      <c r="B28" s="22"/>
+      <c r="C28" s="22"/>
+      <c r="D28" s="22"/>
+      <c r="E28" s="22"/>
+      <c r="F28" s="22"/>
       <c r="G28" s="21"/>
       <c r="H28" s="21"/>
     </row>
-    <row r="29" spans="1:8" ht="120" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A29" s="20" t="s">
-        <v>91</v>
-      </c>
-      <c r="B29" s="22" t="s">
-        <v>35</v>
-      </c>
-      <c r="C29" s="22" t="s">
-        <v>36</v>
-      </c>
-      <c r="D29" s="22" t="s">
-        <v>49</v>
-      </c>
-      <c r="E29" s="22" t="s">
-        <v>71</v>
-      </c>
-      <c r="F29" s="22" t="s">
-        <v>45</v>
-      </c>
+        <v>224</v>
+      </c>
+      <c r="B29" s="22"/>
+      <c r="C29" s="22"/>
+      <c r="D29" s="22"/>
+      <c r="E29" s="22"/>
+      <c r="F29" s="22"/>
       <c r="G29" s="21"/>
       <c r="H29" s="21"/>
     </row>
-    <row r="30" spans="1:8" ht="120" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A30" s="20" t="s">
-        <v>90</v>
-      </c>
-      <c r="B30" s="22" t="s">
-        <v>35</v>
-      </c>
-      <c r="C30" s="22" t="s">
-        <v>36</v>
-      </c>
-      <c r="D30" s="22" t="s">
-        <v>49</v>
-      </c>
-      <c r="E30" s="22" t="s">
-        <v>71</v>
-      </c>
-      <c r="F30" s="22" t="s">
-        <v>45</v>
-      </c>
+        <v>222</v>
+      </c>
+      <c r="B30" s="22"/>
+      <c r="C30" s="22"/>
+      <c r="D30" s="22"/>
+      <c r="E30" s="22"/>
+      <c r="F30" s="22"/>
       <c r="G30" s="21"/>
       <c r="H30" s="21"/>
     </row>
-    <row r="31" spans="1:8" ht="120" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="20" t="s">
-        <v>89</v>
-      </c>
-      <c r="B31" s="22" t="s">
-        <v>35</v>
-      </c>
-      <c r="C31" s="22" t="s">
-        <v>36</v>
-      </c>
-      <c r="D31" s="22" t="s">
-        <v>49</v>
-      </c>
-      <c r="E31" s="22" t="s">
-        <v>71</v>
-      </c>
-      <c r="F31" s="22" t="s">
-        <v>45</v>
-      </c>
+        <v>221</v>
+      </c>
+      <c r="B31" s="22"/>
+      <c r="C31" s="22"/>
+      <c r="D31" s="22"/>
+      <c r="E31" s="22"/>
+      <c r="F31" s="22"/>
       <c r="G31" s="21"/>
       <c r="H31" s="21"/>
     </row>
-    <row r="32" spans="1:8" ht="120" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="20" t="s">
-        <v>88</v>
-      </c>
-      <c r="B32" s="22" t="s">
-        <v>35</v>
-      </c>
-      <c r="C32" s="22" t="s">
-        <v>36</v>
-      </c>
-      <c r="D32" s="22" t="s">
-        <v>49</v>
-      </c>
-      <c r="E32" s="22" t="s">
-        <v>71</v>
-      </c>
-      <c r="F32" s="22" t="s">
-        <v>45</v>
-      </c>
+        <v>220</v>
+      </c>
+      <c r="B32" s="22"/>
+      <c r="C32" s="22"/>
+      <c r="D32" s="22"/>
+      <c r="E32" s="22"/>
+      <c r="F32" s="22"/>
       <c r="G32" s="21"/>
       <c r="H32" s="21"/>
     </row>
     <row r="33" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A33" s="20" t="s">
-        <v>87</v>
+        <v>94</v>
       </c>
       <c r="B33" s="22" t="s">
         <v>35</v>
@@ -18510,7 +18536,7 @@
     </row>
     <row r="34" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A34" s="20" t="s">
-        <v>86</v>
+        <v>93</v>
       </c>
       <c r="B34" s="22" t="s">
         <v>35</v>
@@ -18532,7 +18558,7 @@
     </row>
     <row r="35" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A35" s="20" t="s">
-        <v>85</v>
+        <v>92</v>
       </c>
       <c r="B35" s="22" t="s">
         <v>35</v>
@@ -18554,7 +18580,7 @@
     </row>
     <row r="36" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A36" s="20" t="s">
-        <v>84</v>
+        <v>91</v>
       </c>
       <c r="B36" s="22" t="s">
         <v>35</v>
@@ -18576,7 +18602,7 @@
     </row>
     <row r="37" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A37" s="20" t="s">
-        <v>83</v>
+        <v>90</v>
       </c>
       <c r="B37" s="22" t="s">
         <v>35</v>
@@ -18598,7 +18624,7 @@
     </row>
     <row r="38" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A38" s="20" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
       <c r="B38" s="22" t="s">
         <v>35</v>
@@ -18620,7 +18646,7 @@
     </row>
     <row r="39" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A39" s="20" t="s">
-        <v>81</v>
+        <v>88</v>
       </c>
       <c r="B39" s="22" t="s">
         <v>35</v>
@@ -18642,7 +18668,7 @@
     </row>
     <row r="40" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A40" s="20" t="s">
-        <v>70</v>
+        <v>87</v>
       </c>
       <c r="B40" s="22" t="s">
         <v>35</v>
@@ -18664,7 +18690,7 @@
     </row>
     <row r="41" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A41" s="20" t="s">
-        <v>65</v>
+        <v>86</v>
       </c>
       <c r="B41" s="22" t="s">
         <v>35</v>
@@ -18676,7 +18702,7 @@
         <v>49</v>
       </c>
       <c r="E41" s="22" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="F41" s="22" t="s">
         <v>45</v>
@@ -18686,7 +18712,7 @@
     </row>
     <row r="42" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A42" s="20" t="s">
-        <v>64</v>
+        <v>85</v>
       </c>
       <c r="B42" s="22" t="s">
         <v>35</v>
@@ -18698,7 +18724,7 @@
         <v>49</v>
       </c>
       <c r="E42" s="22" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="F42" s="22" t="s">
         <v>45</v>
@@ -18708,7 +18734,7 @@
     </row>
     <row r="43" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A43" s="20" t="s">
-        <v>62</v>
+        <v>84</v>
       </c>
       <c r="B43" s="22" t="s">
         <v>35</v>
@@ -18720,7 +18746,7 @@
         <v>49</v>
       </c>
       <c r="E43" s="22" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="F43" s="22" t="s">
         <v>45</v>
@@ -18730,7 +18756,7 @@
     </row>
     <row r="44" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A44" s="20" t="s">
-        <v>61</v>
+        <v>83</v>
       </c>
       <c r="B44" s="22" t="s">
         <v>35</v>
@@ -18738,13 +18764,13 @@
       <c r="C44" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="D44" s="21" t="s">
+      <c r="D44" s="22" t="s">
         <v>49</v>
       </c>
-      <c r="E44" s="21" t="s">
-        <v>44</v>
-      </c>
-      <c r="F44" s="21" t="s">
+      <c r="E44" s="22" t="s">
+        <v>71</v>
+      </c>
+      <c r="F44" s="22" t="s">
         <v>45</v>
       </c>
       <c r="G44" s="21"/>
@@ -18752,7 +18778,7 @@
     </row>
     <row r="45" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A45" s="20" t="s">
-        <v>60</v>
+        <v>82</v>
       </c>
       <c r="B45" s="22" t="s">
         <v>35</v>
@@ -18760,13 +18786,13 @@
       <c r="C45" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="D45" s="21" t="s">
+      <c r="D45" s="22" t="s">
         <v>49</v>
       </c>
-      <c r="E45" s="21" t="s">
-        <v>44</v>
-      </c>
-      <c r="F45" s="21" t="s">
+      <c r="E45" s="22" t="s">
+        <v>71</v>
+      </c>
+      <c r="F45" s="22" t="s">
         <v>45</v>
       </c>
       <c r="G45" s="21"/>
@@ -18774,7 +18800,7 @@
     </row>
     <row r="46" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A46" s="20" t="s">
-        <v>59</v>
+        <v>81</v>
       </c>
       <c r="B46" s="22" t="s">
         <v>35</v>
@@ -18782,13 +18808,13 @@
       <c r="C46" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="D46" s="21" t="s">
+      <c r="D46" s="22" t="s">
         <v>49</v>
       </c>
-      <c r="E46" s="21" t="s">
-        <v>44</v>
-      </c>
-      <c r="F46" s="21" t="s">
+      <c r="E46" s="22" t="s">
+        <v>71</v>
+      </c>
+      <c r="F46" s="22" t="s">
         <v>45</v>
       </c>
       <c r="G46" s="21"/>
@@ -18796,7 +18822,7 @@
     </row>
     <row r="47" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A47" s="20" t="s">
-        <v>58</v>
+        <v>70</v>
       </c>
       <c r="B47" s="22" t="s">
         <v>35</v>
@@ -18804,13 +18830,13 @@
       <c r="C47" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="D47" s="21" t="s">
+      <c r="D47" s="22" t="s">
         <v>49</v>
       </c>
-      <c r="E47" s="21" t="s">
-        <v>44</v>
-      </c>
-      <c r="F47" s="21" t="s">
+      <c r="E47" s="22" t="s">
+        <v>71</v>
+      </c>
+      <c r="F47" s="22" t="s">
         <v>45</v>
       </c>
       <c r="G47" s="21"/>
@@ -18818,7 +18844,7 @@
     </row>
     <row r="48" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A48" s="20" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="B48" s="22" t="s">
         <v>35</v>
@@ -18826,13 +18852,13 @@
       <c r="C48" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="D48" s="21" t="s">
+      <c r="D48" s="22" t="s">
         <v>49</v>
       </c>
-      <c r="E48" s="21" t="s">
-        <v>44</v>
-      </c>
-      <c r="F48" s="21" t="s">
+      <c r="E48" s="22" t="s">
+        <v>63</v>
+      </c>
+      <c r="F48" s="22" t="s">
         <v>45</v>
       </c>
       <c r="G48" s="21"/>
@@ -18840,7 +18866,7 @@
     </row>
     <row r="49" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A49" s="20" t="s">
-        <v>48</v>
+        <v>64</v>
       </c>
       <c r="B49" s="22" t="s">
         <v>35</v>
@@ -18848,13 +18874,13 @@
       <c r="C49" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="D49" s="21" t="s">
+      <c r="D49" s="22" t="s">
         <v>49</v>
       </c>
-      <c r="E49" s="21" t="s">
-        <v>44</v>
-      </c>
-      <c r="F49" s="21" t="s">
+      <c r="E49" s="22" t="s">
+        <v>63</v>
+      </c>
+      <c r="F49" s="22" t="s">
         <v>45</v>
       </c>
       <c r="G49" s="21"/>
@@ -18862,7 +18888,7 @@
     </row>
     <row r="50" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A50" s="20" t="s">
-        <v>42</v>
+        <v>62</v>
       </c>
       <c r="B50" s="22" t="s">
         <v>35</v>
@@ -18870,13 +18896,13 @@
       <c r="C50" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="D50" s="21" t="s">
-        <v>43</v>
-      </c>
-      <c r="E50" s="21" t="s">
-        <v>44</v>
-      </c>
-      <c r="F50" s="21" t="s">
+      <c r="D50" s="22" t="s">
+        <v>49</v>
+      </c>
+      <c r="E50" s="22" t="s">
+        <v>63</v>
+      </c>
+      <c r="F50" s="22" t="s">
         <v>45</v>
       </c>
       <c r="G50" s="21"/>
@@ -18884,7 +18910,7 @@
     </row>
     <row r="51" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A51" s="20" t="s">
-        <v>38</v>
+        <v>61</v>
       </c>
       <c r="B51" s="22" t="s">
         <v>35</v>
@@ -18892,27 +18918,43 @@
       <c r="C51" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="D51" s="21"/>
-      <c r="E51" s="21"/>
-      <c r="F51" s="21"/>
+      <c r="D51" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="E51" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="F51" s="21" t="s">
+        <v>45</v>
+      </c>
       <c r="G51" s="21"/>
       <c r="H51" s="21"/>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A52" s="20" t="s">
-        <v>37</v>
-      </c>
-      <c r="B52" s="21"/>
-      <c r="C52" s="21"/>
-      <c r="D52" s="21"/>
-      <c r="E52" s="21"/>
-      <c r="F52" s="21"/>
+        <v>60</v>
+      </c>
+      <c r="B52" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="C52" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="D52" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="E52" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="F52" s="21" t="s">
+        <v>45</v>
+      </c>
       <c r="G52" s="21"/>
       <c r="H52" s="21"/>
     </row>
     <row r="53" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A53" s="20" t="s">
-        <v>34</v>
+        <v>59</v>
       </c>
       <c r="B53" s="22" t="s">
         <v>35</v>
@@ -18920,14 +18962,152 @@
       <c r="C53" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="D53" s="21"/>
-      <c r="E53" s="21"/>
-      <c r="F53" s="21"/>
+      <c r="D53" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="E53" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="F53" s="21" t="s">
+        <v>45</v>
+      </c>
       <c r="G53" s="21"/>
       <c r="H53" s="21"/>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A54" s="19" t="s">
+    <row r="54" spans="1:8" ht="120" x14ac:dyDescent="0.25">
+      <c r="A54" s="20" t="s">
+        <v>58</v>
+      </c>
+      <c r="B54" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="C54" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="D54" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="E54" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="F54" s="21" t="s">
+        <v>45</v>
+      </c>
+      <c r="G54" s="21"/>
+      <c r="H54" s="21"/>
+    </row>
+    <row r="55" spans="1:8" ht="120" x14ac:dyDescent="0.25">
+      <c r="A55" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="B55" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="C55" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="D55" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="E55" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="F55" s="21" t="s">
+        <v>45</v>
+      </c>
+      <c r="G55" s="21"/>
+      <c r="H55" s="21"/>
+    </row>
+    <row r="56" spans="1:8" ht="120" x14ac:dyDescent="0.25">
+      <c r="A56" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="B56" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="C56" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="D56" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="E56" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="F56" s="21" t="s">
+        <v>45</v>
+      </c>
+      <c r="G56" s="21"/>
+      <c r="H56" s="21"/>
+    </row>
+    <row r="57" spans="1:8" ht="120" x14ac:dyDescent="0.25">
+      <c r="A57" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="B57" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="C57" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="D57" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="E57" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="F57" s="21" t="s">
+        <v>45</v>
+      </c>
+      <c r="G57" s="21"/>
+      <c r="H57" s="21"/>
+    </row>
+    <row r="58" spans="1:8" ht="120" x14ac:dyDescent="0.25">
+      <c r="A58" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="B58" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="C58" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="D58" s="21"/>
+      <c r="E58" s="21"/>
+      <c r="F58" s="21"/>
+      <c r="G58" s="21"/>
+      <c r="H58" s="21"/>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A59" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="B59" s="21"/>
+      <c r="C59" s="21"/>
+      <c r="D59" s="21"/>
+      <c r="E59" s="21"/>
+      <c r="F59" s="21"/>
+      <c r="G59" s="21"/>
+      <c r="H59" s="21"/>
+    </row>
+    <row r="60" spans="1:8" ht="120" x14ac:dyDescent="0.25">
+      <c r="A60" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="B60" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="C60" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="D60" s="21"/>
+      <c r="E60" s="21"/>
+      <c r="F60" s="21"/>
+      <c r="G60" s="21"/>
+      <c r="H60" s="21"/>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A61" s="19" t="s">
         <v>32</v>
       </c>
     </row>

</xml_diff>